<commit_message>
more finished animations for Cleyra Dancer "Jeame"
</commit_message>
<xml_diff>
--- a/ProjectSheet.xlsx
+++ b/ProjectSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
   <si>
     <t>Character</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>KingLeo/Baku</t>
+  </si>
+  <si>
+    <t>Puck</t>
   </si>
 </sst>
 </file>
@@ -148,7 +151,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -214,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -232,9 +235,18 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
@@ -252,8 +264,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:K16" displayName="Table1" name="Table1" id="1" totalsRowShown="0">
-  <autoFilter ref="A1:K16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:K17" displayName="Table1" name="Table1" id="1" totalsRowShown="0">
+  <autoFilter ref="A1:K17"/>
   <tableColumns count="11">
     <tableColumn name="Character" id="1" totalsRowLabel="Total"/>
     <tableColumn name="HWS" id="2"/>
@@ -269,7 +281,7 @@
       <totalsRowFormula>Sum</totalsRowFormula>
     </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showColumnStripes="0" showRowStripes="1" showLastColumn="0" showFirstColumn="0"/>
+  <tableStyleInfo name="TableStyleLight1" showColumnStripes="0" showRowStripes="1" showLastColumn="0" showFirstColumn="0"/>
 </table>
 </file>
 
@@ -561,26 +573,26 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="12.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="10.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="33.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="8.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="10.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="33.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="10" width="15.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="8" width="8.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -615,7 +627,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -644,7 +656,7 @@
       <c r="J2" s="3"/>
       <c r="K2" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -673,7 +685,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -702,7 +714,7 @@
       <c r="J4" s="3"/>
       <c r="K4" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -731,7 +743,7 @@
       <c r="J5" s="3"/>
       <c r="K5" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -760,7 +772,7 @@
       <c r="J6" s="3"/>
       <c r="K6" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -789,7 +801,7 @@
       <c r="J7" s="3"/>
       <c r="K7" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
@@ -818,7 +830,7 @@
       <c r="J8" s="3"/>
       <c r="K8" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -847,7 +859,7 @@
       <c r="J9" s="3"/>
       <c r="K9" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -864,7 +876,7 @@
       <c r="J10" s="3"/>
       <c r="K10" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -879,7 +891,7 @@
       <c r="J11" s="3"/>
       <c r="K11" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
@@ -894,7 +906,7 @@
       <c r="J12" s="3"/>
       <c r="K12" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -909,7 +921,7 @@
       <c r="J13" s="3"/>
       <c r="K13" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -924,7 +936,7 @@
       <c r="J14" s="3"/>
       <c r="K14" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
@@ -939,20 +951,35 @@
       <c r="J15" s="3"/>
       <c r="K15" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
       <c r="J16" s="3"/>
-      <c r="K16" s="1"/>
+      <c r="K16" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
+      <c r="A17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
prepping for mikoto and genome
</commit_message>
<xml_diff>
--- a/ProjectSheet.xlsx
+++ b/ProjectSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
   <si>
     <t>Character</t>
   </si>
@@ -34,6 +34,9 @@
     <t>Animation Set</t>
   </si>
   <si>
+    <t>Attack Sequence</t>
+  </si>
+  <si>
     <t>Bone Hierarchy</t>
   </si>
   <si>
@@ -76,13 +79,13 @@
     <t>Sword</t>
   </si>
   <si>
-    <t>Zidane Thief Sword w/ Blank Victory</t>
+    <t>ZidaneTSword_Blank</t>
   </si>
   <si>
     <t>Kohel</t>
   </si>
   <si>
-    <t>Blank w/ Zidane Thief Sword Victory</t>
+    <t>Blank_ZidaneTSword</t>
   </si>
   <si>
     <t>Aria</t>
@@ -91,13 +94,13 @@
     <t>Claws</t>
   </si>
   <si>
-    <t>Zidane Dagger</t>
+    <t>ZidaneDagger</t>
   </si>
   <si>
     <t>Ophelia</t>
   </si>
   <si>
-    <t>Beatrix with Alexandrian Think Victory</t>
+    <t>Beatrix_Alexandrian</t>
   </si>
   <si>
     <t>Dan</t>
@@ -112,28 +115,34 @@
     <t>CleyraDancer</t>
   </si>
   <si>
+    <t>Racket</t>
+  </si>
+  <si>
+    <t>EikoRacket_ThrowDisc</t>
+  </si>
+  <si>
+    <t>Mikoto</t>
+  </si>
+  <si>
     <t>InProgress</t>
   </si>
   <si>
+    <t>Genome</t>
+  </si>
+  <si>
     <t>Ruby</t>
   </si>
   <si>
     <t>Nero</t>
   </si>
   <si>
-    <t>Mikoto</t>
-  </si>
-  <si>
-    <t>Genome</t>
-  </si>
-  <si>
     <t>PurpleGuard</t>
   </si>
   <si>
+    <t>Puck</t>
+  </si>
+  <si>
     <t>KingLeo/Baku</t>
-  </si>
-  <si>
-    <t>Puck</t>
   </si>
 </sst>
 </file>
@@ -156,26 +165,21 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00a933"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -198,26 +202,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF00a933"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF00a933"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF00a933"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF00a933"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -225,28 +214,22 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
@@ -264,24 +247,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:K17" displayName="Table1" name="Table1" id="1" totalsRowShown="0">
-  <autoFilter ref="A1:K17"/>
-  <tableColumns count="11">
-    <tableColumn name="Character" id="1" totalsRowLabel="Total"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:L17" displayName="Table1" name="Table1" id="1" totalsRowShown="0">
+  <autoFilter ref="A1:L17"/>
+  <tableColumns count="12">
+    <tableColumn name="Character" id="1"/>
     <tableColumn name="HWS" id="2"/>
     <tableColumn name="ID" id="3"/>
     <tableColumn name="Face ID" id="4"/>
     <tableColumn name="Weapon" id="5"/>
     <tableColumn name="Animation Set" id="6"/>
-    <tableColumn name="Bone Hierarchy" id="7"/>
-    <tableColumn name="Portrait" id="8"/>
-    <tableColumn name="Stats Balanced" id="9"/>
-    <tableColumn name="Skills Set1" id="10"/>
-    <tableColumn name="Notes" id="11" totalsRowFunction="custom">
-      <totalsRowFormula>Sum</totalsRowFormula>
+    <tableColumn name="Attack Sequence" id="7"/>
+    <tableColumn name="Bone Hierarchy" id="8"/>
+    <tableColumn name="Portrait" id="9"/>
+    <tableColumn name="Stats Balanced" id="10"/>
+    <tableColumn name="Skills Set" id="11"/>
+    <tableColumn name="Notes" id="12" totalsRowFunction="custom">
+      <totalsRowFormula>id="12" name="Not</totalsRowFormula>
     </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showColumnStripes="0" showRowStripes="1" showLastColumn="0" showFirstColumn="0"/>
+  <tableStyleInfo name="TableStyleLight1" showColumnStripes="0" showRowStripes="0" showLastColumn="0" showFirstColumn="0"/>
 </table>
 </file>
 
@@ -573,26 +557,27 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="12.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="10.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="33.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="10" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="8.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="10.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="5.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="8.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="20.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="14.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="7" width="8.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -614,7 +599,7 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -626,13 +611,16 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="5">
         <v>12</v>
@@ -641,27 +629,30 @@
         <v>13</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="G2" s="5">
+        <v>104</v>
+      </c>
       <c r="H2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="5">
         <v>13</v>
@@ -670,27 +661,30 @@
         <v>14</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>12</v>
+      <c r="G3" s="5">
+        <v>112</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="5">
         <v>14</v>
@@ -699,27 +693,30 @@
         <v>15</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>12</v>
+      <c r="G4" s="5">
+        <v>107</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="5">
         <v>15</v>
@@ -728,27 +725,30 @@
         <v>16</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>12</v>
+        <v>21</v>
+      </c>
+      <c r="G5" s="5">
+        <v>101</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="5">
         <v>16</v>
@@ -757,27 +757,30 @@
         <v>17</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>12</v>
+        <v>23</v>
+      </c>
+      <c r="G6" s="5">
+        <v>116</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5">
         <v>17</v>
@@ -786,27 +789,30 @@
         <v>18</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>12</v>
+        <v>26</v>
+      </c>
+      <c r="G7" s="5">
+        <v>100</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" s="5">
         <v>18</v>
@@ -815,27 +821,30 @@
         <v>19</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>12</v>
+        <v>28</v>
+      </c>
+      <c r="G8" s="5">
+        <v>118</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" s="5">
         <v>19</v>
@@ -844,142 +853,169 @@
         <v>20</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>12</v>
+        <v>31</v>
+      </c>
+      <c r="G9" s="5">
+        <v>115</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="1"/>
+      <c r="B10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="5">
+        <v>20</v>
+      </c>
+      <c r="D10" s="5">
+        <v>21</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="5">
+        <v>2000</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="1"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+        <v>37</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="1"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="1"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="1"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+        <v>40</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="1"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
+      <c r="A16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="6"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
       <c r="A17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="1"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
prepping Gerome the Genome with Lani animations
</commit_message>
<xml_diff>
--- a/ProjectSheet.xlsx
+++ b/ProjectSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
   <si>
     <t>Character</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>InProgress</t>
+  </si>
+  <si>
+    <t>Throwing Knife</t>
+  </si>
+  <si>
+    <t>Zidane Dagger</t>
   </si>
   <si>
     <t>Genome</t>
@@ -150,7 +156,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,12 +167,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -206,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -214,23 +214,14 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -563,18 +554,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="10.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="5.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="8.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="20.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="14.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="7" width="8.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="10.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="5.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="8.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="20.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="5" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="4" width="14.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="4" width="8.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -596,10 +587,10 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -619,402 +610,412 @@
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="5">
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3">
         <v>12</v>
       </c>
-      <c r="D2" s="5">
-        <v>13</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="3">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="3">
         <v>104</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="4" t="s">
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J2" s="1"/>
-      <c r="K2" s="4"/>
+      <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="5">
-        <v>13</v>
-      </c>
-      <c r="D3" s="5">
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3">
         <v>14</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="3">
         <v>112</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="4" t="s">
+      <c r="H3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J3" s="1"/>
-      <c r="K3" s="4"/>
+      <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3">
         <v>14</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>15</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="3">
         <v>107</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="4" t="s">
+      <c r="H4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J4" s="1"/>
-      <c r="K4" s="4"/>
+      <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="5">
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="3">
         <v>15</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>16</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="3">
         <v>101</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="4" t="s">
+      <c r="H5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J5" s="1"/>
-      <c r="K5" s="4"/>
+      <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="5">
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3">
         <v>16</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="3">
         <v>17</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="3">
         <v>116</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="4" t="s">
+      <c r="H6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J6" s="1"/>
-      <c r="K6" s="4"/>
+      <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3">
         <v>17</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="3">
         <v>18</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="3">
         <v>100</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="4" t="s">
+      <c r="H7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J7" s="1"/>
-      <c r="K7" s="4"/>
+      <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="5">
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3">
         <v>18</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="3">
         <v>19</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="3">
         <v>118</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="4" t="s">
+      <c r="H8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J8" s="1"/>
-      <c r="K8" s="4"/>
+      <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="5">
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3">
         <v>19</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="3">
         <v>20</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="3">
         <v>115</v>
       </c>
-      <c r="H9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="4" t="s">
+      <c r="H9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J9" s="1"/>
-      <c r="K9" s="4"/>
+      <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="5">
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3">
         <v>20</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="3">
         <v>21</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="3">
         <v>2000</v>
       </c>
-      <c r="H10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="4" t="s">
+      <c r="H10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J10" s="1"/>
-      <c r="K10" s="4"/>
+      <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="C11" s="3">
+        <v>21</v>
+      </c>
+      <c r="D11" s="3">
+        <v>22</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="3">
+        <v>2001</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="4"/>
+      <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="4"/>
+      <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="4"/>
+      <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="4"/>
+      <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-      <c r="K15" s="4"/>
+      <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
       <c r="A17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="4"/>
+      <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more animation stuff for Genome and also exporting Steiner animations
</commit_message>
<xml_diff>
--- a/ProjectSheet.xlsx
+++ b/ProjectSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
   <si>
     <t>Character</t>
   </si>
@@ -124,16 +124,19 @@
     <t>Mikoto</t>
   </si>
   <si>
+    <t>Throwing Knife</t>
+  </si>
+  <si>
+    <t>Zidane Dagger</t>
+  </si>
+  <si>
+    <t>Genome</t>
+  </si>
+  <si>
     <t>InProgress</t>
   </si>
   <si>
-    <t>Throwing Knife</t>
-  </si>
-  <si>
-    <t>Zidane Dagger</t>
-  </si>
-  <si>
-    <t>Genome</t>
+    <t>Lani_ZidaneDagger</t>
   </si>
   <si>
     <t>Ruby</t>
@@ -899,7 +902,7 @@
         <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="C11" s="3">
         <v>21</v>
@@ -908,10 +911,10 @@
         <v>22</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="G11" s="3">
         <v>2001</v>
@@ -924,23 +927,37 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="C12" s="3">
+        <v>22</v>
+      </c>
+      <c r="D12" s="3">
+        <v>23</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="G12" s="2"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
@@ -956,7 +973,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
@@ -972,7 +989,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
@@ -988,7 +1005,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
@@ -1004,7 +1021,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
       <c r="A17" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="2"/>

</xml_diff>

<commit_message>
finished Baku animations for now
</commit_message>
<xml_diff>
--- a/ProjectSheet.xlsx
+++ b/ProjectSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="47">
   <si>
     <t>Character</t>
   </si>
@@ -133,25 +133,28 @@
     <t>Genome</t>
   </si>
   <si>
-    <t>InProgress</t>
-  </si>
-  <si>
     <t>Lani_ZidaneDagger</t>
   </si>
   <si>
     <t>Ruby</t>
   </si>
   <si>
-    <t>Nero</t>
-  </si>
-  <si>
-    <t>PurpleGuard</t>
+    <t>Ruby_DaggerRacket</t>
   </si>
   <si>
     <t>Puck</t>
   </si>
   <si>
+    <t>Rod</t>
+  </si>
+  <si>
+    <t>Puck_Vivi</t>
+  </si>
+  <si>
     <t>KingLeo/Baku</t>
+  </si>
+  <si>
+    <t>Baku_BakuEnemy_KingLeo_Steiner</t>
   </si>
 </sst>
 </file>
@@ -224,7 +227,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -241,8 +244,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:L17" displayName="Table1" name="Table1" id="1" totalsRowShown="0">
-  <autoFilter ref="A1:L17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:L15" displayName="Table1" name="Table1" id="1" totalsRowShown="0">
+  <autoFilter ref="A1:L15"/>
   <tableColumns count="12">
     <tableColumn name="Character" id="1"/>
     <tableColumn name="HWS" id="2"/>
@@ -551,7 +554,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -562,7 +565,7 @@
     <col min="3" max="3" style="5" width="5.719285714285714" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="5" width="8.290714285714287" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="20.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="32.57642857142857" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="5" width="15.719285714285713" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="4" width="14.43357142857143" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="4" width="8.576428571428572" customWidth="1" bestFit="1"/>
@@ -919,7 +922,9 @@
       <c r="G11" s="3">
         <v>2001</v>
       </c>
-      <c r="H11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -930,7 +935,7 @@
         <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="C12" s="3">
         <v>22</v>
@@ -942,9 +947,11 @@
         <v>18</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="G12" s="3">
+        <v>107</v>
+      </c>
       <c r="H12" s="1" t="s">
         <v>13</v>
       </c>
@@ -957,16 +964,32 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="3">
+        <v>23</v>
+      </c>
+      <c r="D13" s="3">
+        <v>24</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="G13" s="3">
+        <v>104</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -975,65 +998,65 @@
       <c r="A14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3">
+        <v>24</v>
+      </c>
+      <c r="D14" s="3">
+        <v>25</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="3">
+        <v>102</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
       <c r="A15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="3">
+        <v>25</v>
+      </c>
+      <c r="D15" s="3">
+        <v>26</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="3">
+        <v>2002</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
-      <c r="A17" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>